<commit_message>
Subindo versões finais dos arquivos
</commit_message>
<xml_diff>
--- a/Arq Comp/analytics.xlsx
+++ b/Arq Comp/analytics.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Documents\git\projeto_Pi\Arq Comp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicol\Documents\Bandtec\Github\projeto_Pi\Arq Comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{FDDC21F6-B00F-4A13-B46A-978E6BFF21E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C9041502-078F-4A4E-8500-888B3E82AE48}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AF5865-D143-4693-B2D7-62E8B0063C0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CE4437CC-FF5A-4486-9164-9D4E885DA380}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CE4437CC-FF5A-4486-9164-9D4E885DA380}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -100,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,7 +273,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -572,10 +572,10 @@
   <dimension ref="A1:AC32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="V18" sqref="A13:V18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -587,7 +587,7 @@
     <col min="20" max="20" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -675,7 +675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -749,7 +749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -839,7 +839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -859,7 +859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -879,7 +879,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -899,7 +899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -919,7 +919,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -939,7 +939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -959,7 +959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -979,7 +979,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -999,7 +999,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>14</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>15</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>16</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="28">
         <v>21</v>
       </c>
@@ -1199,28 +1199,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U27" s="1"/>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U28" s="1"/>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U29" s="1"/>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U32" s="1"/>
     </row>
   </sheetData>
@@ -1230,6 +1230,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A5FC0246A07B443A05063C8EB2AC7D8" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4044185caad13901db6ed9cf027cb62e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8061e086-846d-4709-83ef-f95cce98977c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ef145caafaa4d071a09fcfea9b85fcfc" ns3:_="">
     <xsd:import namespace="8061e086-846d-4709-83ef-f95cce98977c"/>
@@ -1379,29 +1394,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC080077-ED7F-44D9-8DF2-81C40B798909}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74BE4089-E92A-4A6E-9EE3-594E92CD1D83}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4890F991-0C9A-40B0-8E63-EE6519E5CF2F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4890F991-0C9A-40B0-8E63-EE6519E5CF2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74BE4089-E92A-4A6E-9EE3-594E92CD1D83}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC080077-ED7F-44D9-8DF2-81C40B798909}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8061e086-846d-4709-83ef-f95cce98977c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>